<commit_message>
more tests on ebay
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/test_data.xlsx
+++ b/com.ebay/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikto\IdeaProjects\SeleniumBootcamp\com.ebay\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32C6EC2-D962-4417-8088-0B9803ABB674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401820C1-D752-4E81-82EB-7BC9CA3FA5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2076" yWindow="1728" windowWidth="17280" windowHeight="8880" xr2:uid="{6CC8E123-50E6-47AC-A365-0051B47EAF32}"/>
+    <workbookView xWindow="2076" yWindow="1728" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{6CC8E123-50E6-47AC-A365-0051B47EAF32}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchItems" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchItem" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>yeezy</t>
   </si>
@@ -398,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B33AC-3DDA-4E51-A8E2-2F00F2DE94E6}">
   <dimension ref="A2:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -422,4 +423,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F404D7-7A8A-4D7C-95B7-A1CFCA85A4A6}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>